<commit_message>
updating the selenium framework
</commit_message>
<xml_diff>
--- a/excel_datadriven_source.xlsx
+++ b/excel_datadriven_source.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>Testcases</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>qwe1</t>
+  </si>
+  <si>
+    <t>RowSelection</t>
   </si>
 </sst>
 </file>
@@ -562,9 +565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -573,7 +574,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>

</xml_diff>